<commit_message>
added more magnet data for different heights and added data on Vdroop where the magnet running pulls down the phototransistor value
</commit_message>
<xml_diff>
--- a/Lab2/Part1/MagnetData.xlsx
+++ b/Lab2/Part1/MagnetData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>stand height (mm)</t>
   </si>
@@ -28,16 +28,53 @@
   </si>
   <si>
     <t>Voltage to lift (V)</t>
+  </si>
+  <si>
+    <t>height of low part of magnet (mm)</t>
+  </si>
+  <si>
+    <t>depth of depression in magnet (mm)</t>
+  </si>
+  <si>
+    <t>Washer height (mm)</t>
+  </si>
+  <si>
+    <t>note that these voltage are highly sensitive to the relative position of the support to the magnet, needs to be directly beneath or the torque exerted tips it a bit, raising up and letting it grab it</t>
+  </si>
+  <si>
+    <t>Vdroop in transistor</t>
+  </si>
+  <si>
+    <t>Magnet V</t>
+  </si>
+  <si>
+    <t>note that really only goes as low as 9.906 V with loading</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -60,13 +97,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="9">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -396,18 +449,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:B9"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="24.5" customWidth="1"/>
+    <col min="1" max="1" width="31.6640625" customWidth="1"/>
+    <col min="4" max="4" width="19.1640625" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2">
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1">
+        <v>1.23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1">
+        <v>1.43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>129.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -415,48 +492,292 @@
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>1</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>0</v>
       </c>
       <c r="B6">
         <v>1.74</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="F6">
+        <v>0.2</v>
+      </c>
+      <c r="H6">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="K6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7">
         <v>0</v>
       </c>
       <c r="B7">
         <v>1.73</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="F7">
+        <v>0.3</v>
+      </c>
+      <c r="H7">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8">
         <v>0</v>
       </c>
       <c r="B8">
         <v>1.7</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="F8">
+        <v>0.4</v>
+      </c>
+      <c r="H8">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9">
         <v>0</v>
       </c>
       <c r="B9">
         <v>1.74</v>
       </c>
+      <c r="F9">
+        <v>0.5</v>
+      </c>
+      <c r="H9">
+        <v>3.2000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10">
+        <f>-2*E1</f>
+        <v>-2.86</v>
+      </c>
+      <c r="B10">
+        <v>0.74</v>
+      </c>
+      <c r="F10">
+        <v>0.6</v>
+      </c>
+      <c r="H10">
+        <v>3.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11">
+        <f>-1 * E1</f>
+        <v>-1.43</v>
+      </c>
+      <c r="B11">
+        <v>1.17</v>
+      </c>
+      <c r="F11">
+        <v>0.7</v>
+      </c>
+      <c r="H11">
+        <v>4.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12">
+        <v>-1</v>
+      </c>
+      <c r="B12">
+        <v>1.349</v>
+      </c>
+      <c r="F12">
+        <v>0.8</v>
+      </c>
+      <c r="H12">
+        <v>5.3999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13">
+        <v>-0.5</v>
+      </c>
+      <c r="B13">
+        <v>1.5649999999999999</v>
+      </c>
+      <c r="F13">
+        <v>0.9</v>
+      </c>
+      <c r="H13">
+        <v>6.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>1.74</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>6.8000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15">
+        <v>0.5</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="F15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H15">
+        <v>7.1999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16">
+        <f>1.43-0.5</f>
+        <v>0.92999999999999994</v>
+      </c>
+      <c r="B16">
+        <v>2.25</v>
+      </c>
+      <c r="F16">
+        <v>1.2</v>
+      </c>
+      <c r="H16">
+        <v>8.1000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="6:8">
+      <c r="F17">
+        <v>1.3</v>
+      </c>
+      <c r="H17">
+        <v>8.5999999999999993E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="6:8">
+      <c r="F18">
+        <v>1.4</v>
+      </c>
+      <c r="H18">
+        <v>8.2000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="6:8">
+      <c r="F19">
+        <v>1.5</v>
+      </c>
+      <c r="H19">
+        <v>8.7999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="6:8">
+      <c r="F20">
+        <v>1.6</v>
+      </c>
+      <c r="H20">
+        <v>8.8999999999999996E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="6:8">
+      <c r="F21">
+        <v>1.7</v>
+      </c>
+      <c r="H21">
+        <v>9.1999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="6:8">
+      <c r="F22">
+        <v>1.8</v>
+      </c>
+      <c r="H22">
+        <v>9.4E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="6:8">
+      <c r="F23">
+        <v>1.9</v>
+      </c>
+      <c r="H23">
+        <v>9.4E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="6:8">
+      <c r="F24">
+        <v>2</v>
+      </c>
+      <c r="H24">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="6:8">
+      <c r="F25">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H25">
+        <v>9.7000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="6:8">
+      <c r="F26">
+        <v>2.4</v>
+      </c>
+      <c r="H26">
+        <v>9.8000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="6:8">
+      <c r="F27">
+        <v>2.6</v>
+      </c>
+      <c r="H27">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="6:8">
+      <c r="F28">
+        <v>2.8</v>
+      </c>
+      <c r="H28">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="29" spans="6:8">
+      <c r="F29">
+        <v>3</v>
+      </c>
+      <c r="H29">
+        <v>0.96499999999999997</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
added correct math stuff
</commit_message>
<xml_diff>
--- a/Lab2/Part1/MagnetData.xlsx
+++ b/Lab2/Part1/MagnetData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>stand height (mm)</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>note that really only goes as low as 9.906 V with loading</t>
+  </si>
+  <si>
+    <t>x (mm)</t>
   </si>
 </sst>
 </file>
@@ -97,8 +100,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -111,20 +118,523 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Voltage to Lift</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> vs height </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.106893637723202"/>
+                  <c:y val="-0.162445415931841"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$10:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>-2.86</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1.43</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.93</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$10:$D$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.17</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.349</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.565</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.74</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2141671656"/>
+        <c:axId val="2053392136"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2141671656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Displacement from stand height (mm)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2053392136"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2053392136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Voltage to Lift (V)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2141671656"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Voltage to Lift</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> vs height </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.106893637723202"/>
+                  <c:y val="-0.162445415931841"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$10:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>6.870000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.299999999999993</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.73</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.23</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.73</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.23</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.66000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$10:$D$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.17</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.349</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.565</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.74</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2136234216"/>
+        <c:axId val="-2133174728"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2136234216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>X (mm)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2133174728"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2133174728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Voltage to Lift (V)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2136234216"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -451,13 +961,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="31.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
     <col min="4" max="4" width="19.1640625" customWidth="1"/>
     <col min="5" max="5" width="12.83203125" customWidth="1"/>
   </cols>
@@ -497,6 +1008,9 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
         <v>2</v>
       </c>
       <c r="F5" t="s">
@@ -511,6 +1025,10 @@
         <v>0</v>
       </c>
       <c r="B6">
+        <f>(129.5 - (122 + 12.7/2 +A6))</f>
+        <v>1.1500000000000057</v>
+      </c>
+      <c r="D6">
         <v>1.74</v>
       </c>
       <c r="F6">
@@ -528,6 +1046,10 @@
         <v>0</v>
       </c>
       <c r="B7">
+        <f t="shared" ref="B7:B16" si="0">(129.5 - (122 + 12.7/2 +A7))</f>
+        <v>1.1500000000000057</v>
+      </c>
+      <c r="D7">
         <v>1.73</v>
       </c>
       <c r="F7">
@@ -542,6 +1064,10 @@
         <v>0</v>
       </c>
       <c r="B8">
+        <f t="shared" si="0"/>
+        <v>1.1500000000000057</v>
+      </c>
+      <c r="D8">
         <v>1.7</v>
       </c>
       <c r="F8">
@@ -556,6 +1082,10 @@
         <v>0</v>
       </c>
       <c r="B9">
+        <f t="shared" si="0"/>
+        <v>1.1500000000000057</v>
+      </c>
+      <c r="D9">
         <v>1.74</v>
       </c>
       <c r="F9">
@@ -571,6 +1101,10 @@
         <v>-2.86</v>
       </c>
       <c r="B10">
+        <f>A10-121+129.5+1.23</f>
+        <v>6.870000000000001</v>
+      </c>
+      <c r="D10">
         <v>0.74</v>
       </c>
       <c r="F10">
@@ -586,6 +1120,10 @@
         <v>-1.43</v>
       </c>
       <c r="B11">
+        <f t="shared" ref="B11:B16" si="1">A11-121+129.5+1.23</f>
+        <v>8.2999999999999936</v>
+      </c>
+      <c r="D11">
         <v>1.17</v>
       </c>
       <c r="F11">
@@ -600,6 +1138,10 @@
         <v>-1</v>
       </c>
       <c r="B12">
+        <f t="shared" si="1"/>
+        <v>8.73</v>
+      </c>
+      <c r="D12">
         <v>1.349</v>
       </c>
       <c r="F12">
@@ -614,6 +1156,10 @@
         <v>-0.5</v>
       </c>
       <c r="B13">
+        <f t="shared" si="1"/>
+        <v>9.23</v>
+      </c>
+      <c r="D13">
         <v>1.5649999999999999</v>
       </c>
       <c r="F13">
@@ -628,6 +1174,10 @@
         <v>0</v>
       </c>
       <c r="B14">
+        <f t="shared" si="1"/>
+        <v>9.73</v>
+      </c>
+      <c r="D14">
         <v>1.74</v>
       </c>
       <c r="F14">
@@ -642,6 +1192,10 @@
         <v>0.5</v>
       </c>
       <c r="B15">
+        <f t="shared" si="1"/>
+        <v>10.23</v>
+      </c>
+      <c r="D15">
         <v>2</v>
       </c>
       <c r="F15">
@@ -657,6 +1211,10 @@
         <v>0.92999999999999994</v>
       </c>
       <c r="B16">
+        <f t="shared" si="1"/>
+        <v>10.660000000000007</v>
+      </c>
+      <c r="D16">
         <v>2.25</v>
       </c>
       <c r="F16">
@@ -759,7 +1317,7 @@
         <v>2.8</v>
       </c>
       <c r="H28">
-        <v>0.97</v>
+        <v>9.7000000000000003E-2</v>
       </c>
     </row>
     <row r="29" spans="6:8">
@@ -767,17 +1325,18 @@
         <v>3</v>
       </c>
       <c r="H29">
-        <v>0.96499999999999997</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34" t="s">
+        <v>9.6500000000000002E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="5:5">
+      <c r="E34" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
added a plot vs x to help us out
</commit_message>
<xml_diff>
--- a/Lab2/Part1/MagnetData.xlsx
+++ b/Lab2/Part1/MagnetData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22624"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28280" tabRatio="500"/>
+    <workbookView xWindow="1640" yWindow="2260" windowWidth="27580" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -269,11 +269,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2141671656"/>
-        <c:axId val="2053392136"/>
+        <c:axId val="2119688776"/>
+        <c:axId val="2119694296"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2141671656"/>
+        <c:axId val="2119688776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -302,12 +302,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2053392136"/>
+        <c:crossAx val="2119694296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2053392136"/>
+        <c:axId val="2119694296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -337,7 +337,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2141671656"/>
+        <c:crossAx val="2119688776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -485,11 +485,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2136234216"/>
-        <c:axId val="-2133174728"/>
+        <c:axId val="2119919176"/>
+        <c:axId val="2119924520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2136234216"/>
+        <c:axId val="2119919176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -518,12 +518,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2133174728"/>
+        <c:crossAx val="2119924520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2133174728"/>
+        <c:axId val="2119924520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -553,7 +553,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2136234216"/>
+        <c:crossAx val="2119919176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -961,8 +961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1025,7 +1025,7 @@
         <v>0</v>
       </c>
       <c r="B6">
-        <f t="shared" ref="B6:B9" si="0">A6-121+129.5+1.23-12.7/2</f>
+        <f>A6-121+129.5+1.23-12.7/2</f>
         <v>3.3800000000000008</v>
       </c>
       <c r="D6">
@@ -1046,7 +1046,7 @@
         <v>0</v>
       </c>
       <c r="B7">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="B6:B9" si="0">A7-121+129.5+1.23-12.7/2</f>
         <v>3.3800000000000008</v>
       </c>
       <c r="D7">

</xml_diff>